<commit_message>
Comment added in fRasterCalcs, updated naming conventions and list creation in cRecruitmentCriteria, created methods for determining analysis periods, creating q_mobile and bed preparation rasters, and sub-directory for year-of-interest with into.txt file. Additional build out of gui.
</commit_message>
<xml_diff>
--- a/RiparianRecruitment/.templates/recruitment_criteria.xlsx
+++ b/RiparianRecruitment/.templates/recruitment_criteria.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Common name</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Lethal inundation</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -802,14 +805,14 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D24"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="7"/>
-    <col min="3" max="3" width="18.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.88671875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -818,6 +821,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -827,6 +831,9 @@
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="D2" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -836,6 +843,9 @@
       <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
@@ -845,6 +855,9 @@
       <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -854,6 +867,9 @@
       <c r="C5" s="19" t="s">
         <v>9</v>
       </c>
+      <c r="D5" s="19" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -863,6 +879,9 @@
       <c r="C6" s="15">
         <v>44331</v>
       </c>
+      <c r="D6" s="15">
+        <v>44331</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -872,6 +891,9 @@
       <c r="C7" s="23">
         <v>44378</v>
       </c>
+      <c r="D7" s="23">
+        <v>44378</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
@@ -883,6 +905,9 @@
       <c r="C8" s="22">
         <v>2</v>
       </c>
+      <c r="D8" s="22">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
@@ -890,6 +915,7 @@
       </c>
       <c r="B9" s="31"/>
       <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
@@ -899,6 +925,9 @@
       <c r="C10" s="16">
         <v>4.7E-2</v>
       </c>
+      <c r="D10" s="16">
+        <v>4.7E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
@@ -908,6 +937,9 @@
       <c r="C11" s="16">
         <v>0.03</v>
       </c>
+      <c r="D11" s="16">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
@@ -917,6 +949,9 @@
       <c r="C12" s="16">
         <v>0</v>
       </c>
+      <c r="D12" s="16">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
@@ -924,6 +959,7 @@
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
@@ -935,6 +971,9 @@
       <c r="C14" s="17">
         <v>2.5</v>
       </c>
+      <c r="D14" s="17">
+        <v>2.5</v>
+      </c>
       <c r="E14" s="25"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -947,6 +986,9 @@
       <c r="C15" s="17">
         <v>5</v>
       </c>
+      <c r="D15" s="17">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
@@ -958,15 +1000,19 @@
       <c r="C16" s="17">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="21"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>23</v>
       </c>
@@ -976,8 +1022,11 @@
       <c r="C18" s="17">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>27</v>
       </c>
@@ -987,8 +1036,11 @@
       <c r="C19" s="17">
         <v>101</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" s="17">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>28</v>
       </c>
@@ -998,15 +1050,19 @@
       <c r="C20" s="17">
         <v>201</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" s="17">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="31"/>
       <c r="C21" s="21"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="21"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>29</v>
       </c>
@@ -1016,8 +1072,11 @@
       <c r="C22" s="17">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>30</v>
       </c>
@@ -1027,8 +1086,11 @@
       <c r="C23" s="17">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>31</v>
       </c>
@@ -1036,6 +1098,9 @@
         <v>20</v>
       </c>
       <c r="C24" s="18">
+        <v>29</v>
+      </c>
+      <c r="D24" s="18">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated recession rate method to create mortality coefficient raster, added criteria to cRecrtuitmentCriteria
</commit_message>
<xml_diff>
--- a/RiparianRecruitment/.templates/recruitment_criteria.xlsx
+++ b/RiparianRecruitment/.templates/recruitment_criteria.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Common name</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>TEST</t>
+  </si>
+  <si>
+    <t>Base flow period starts</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -522,6 +525,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -872,7 +876,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="28"/>
@@ -884,7 +888,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="28"/>
@@ -896,211 +900,223 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="23">
+        <v>44454</v>
+      </c>
+      <c r="D8" s="23">
+        <v>44454</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B9" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C9" s="22">
         <v>2</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D9" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="16">
-        <v>4.7E-2</v>
-      </c>
-      <c r="D10" s="16">
-        <v>4.7E-2</v>
-      </c>
+      <c r="B10" s="31"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="28"/>
       <c r="C11" s="16">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D11" s="16">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="16">
         <v>0.03</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D12" s="16">
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="16">
+      <c r="B13" s="32"/>
+      <c r="C13" s="16">
         <v>0</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D13" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="17">
-        <v>2.5</v>
-      </c>
-      <c r="D14" s="17">
-        <v>2.5</v>
-      </c>
-      <c r="E14" s="25"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="17">
+        <v>2.5</v>
+      </c>
+      <c r="D15" s="17">
+        <v>2.5</v>
+      </c>
+      <c r="E15" s="25"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="17">
         <v>5</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D16" s="17">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B17" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C17" s="17">
         <v>10</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D17" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="17">
-        <v>0</v>
-      </c>
-      <c r="D18" s="17">
-        <v>0</v>
-      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B19" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="17">
+        <v>0</v>
+      </c>
+      <c r="D19" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="17">
         <v>101</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D20" s="17">
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B21" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C21" s="17">
         <v>201</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D21" s="17">
         <v>201</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="17">
-        <v>0</v>
-      </c>
-      <c r="D22" s="17">
-        <v>0</v>
-      </c>
+      <c r="B22" s="31"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="17">
+        <v>0</v>
+      </c>
+      <c r="D23" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="17">
         <v>15</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D24" s="17">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B25" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C25" s="18">
         <v>29</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D25" s="18">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added inundation and scour&burial survival raster methods, recruitment potential raster method, and area totals
</commit_message>
<xml_diff>
--- a/RiparianRecruitment/.templates/recruitment_criteria.xlsx
+++ b/RiparianRecruitment/.templates/recruitment_criteria.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Common name</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Recession rate criteria</t>
   </si>
   <si>
-    <t>cm</t>
-  </si>
-  <si>
     <t>cm/day</t>
   </si>
   <si>
@@ -75,12 +72,6 @@
     <t>UNITS</t>
   </si>
   <si>
-    <t>Elevation criteria</t>
-  </si>
-  <si>
-    <t>Inundation criteria</t>
-  </si>
-  <si>
     <t>days</t>
   </si>
   <si>
@@ -90,27 +81,12 @@
     <t>Bed preparation period</t>
   </si>
   <si>
-    <t>Favorable elevation</t>
-  </si>
-  <si>
-    <t>Favorable rate</t>
-  </si>
-  <si>
     <t>Stressful rate</t>
   </si>
   <si>
     <t>Lethal rate</t>
   </si>
   <si>
-    <t>Stressful elevation</t>
-  </si>
-  <si>
-    <t>Lethal elevation</t>
-  </si>
-  <si>
-    <t>Favorable inundation</t>
-  </si>
-  <si>
     <t>Stressful inundation</t>
   </si>
   <si>
@@ -121,6 +97,9 @@
   </si>
   <si>
     <t>Base flow period starts</t>
+  </si>
+  <si>
+    <t>Inundation criteria (partial or complete shoot inundation)</t>
   </si>
 </sst>
 </file>
@@ -500,7 +479,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -526,6 +504,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -806,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -819,31 +800,31 @@
     <col min="3" max="4" width="18.88671875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
-      <c r="B1" s="26" t="s">
-        <v>17</v>
+      <c r="B1" s="25" t="s">
+        <v>16</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
@@ -851,11 +832,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
@@ -863,11 +844,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="19" t="s">
         <v>9</v>
       </c>
@@ -875,11 +856,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="28"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="15">
         <v>44331</v>
       </c>
@@ -887,11 +868,11 @@
         <v>44331</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="28"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="23">
         <v>44378</v>
       </c>
@@ -899,11 +880,11 @@
         <v>44378</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="28"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="27"/>
       <c r="C8" s="23">
         <v>44454</v>
       </c>
@@ -911,12 +892,12 @@
         <v>44454</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>18</v>
       </c>
       <c r="C9" s="22">
         <v>2</v>
@@ -925,43 +906,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="31"/>
+        <v>12</v>
+      </c>
+      <c r="B10" s="30"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="28"/>
+        <v>13</v>
+      </c>
+      <c r="B11" s="27"/>
       <c r="C11" s="16">
         <v>4.7E-2</v>
       </c>
       <c r="D11" s="16">
-        <v>4.7E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="28"/>
+        <v>14</v>
+      </c>
+      <c r="B12" s="27"/>
       <c r="C12" s="16">
         <v>0.03</v>
       </c>
       <c r="D12" s="16">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="32"/>
+        <v>15</v>
+      </c>
+      <c r="B13" s="31"/>
       <c r="C13" s="16">
         <v>0</v>
       </c>
@@ -969,155 +950,76 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="33"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>11</v>
       </c>
       <c r="C15" s="17">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="D15" s="17">
-        <v>2.5</v>
-      </c>
-      <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>11</v>
       </c>
       <c r="C16" s="17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D16" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="17">
-        <v>10</v>
-      </c>
-      <c r="D17" s="17">
-        <v>10</v>
-      </c>
+      <c r="B17" s="30"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="A18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="17">
+        <v>14</v>
+      </c>
+      <c r="D18" s="17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="17">
-        <v>0</v>
-      </c>
-      <c r="D19" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="17">
-        <v>101</v>
-      </c>
-      <c r="D20" s="17">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="18">
         <v>28</v>
       </c>
-      <c r="B21" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="17">
-        <v>201</v>
-      </c>
-      <c r="D21" s="17">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="17">
-        <v>0</v>
-      </c>
-      <c r="D23" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="17">
-        <v>15</v>
-      </c>
-      <c r="D24" s="17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="18">
-        <v>29</v>
-      </c>
-      <c r="D25" s="18">
-        <v>29</v>
+      <c r="D19" s="18">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed code to run from cRecruitmentPotential
- removed code to run cRecruitmentPotential from interpreter
- updated recruitment_criteria worksheet to include criteria
for assessing bed prep in graded areas
</commit_message>
<xml_diff>
--- a/RiparianRecruitment/.templates/recruitment_criteria.xlsx
+++ b/RiparianRecruitment/.templates/recruitment_criteria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17496" windowHeight="6432"/>
   </bookViews>
   <sheets>
     <sheet name="recruitment" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Common name</t>
   </si>
@@ -93,13 +93,22 @@
     <t>Lethal inundation</t>
   </si>
   <si>
+    <t>Base flow period starts</t>
+  </si>
+  <si>
+    <t>Inundation criteria (partial or complete shoot inundation)</t>
+  </si>
+  <si>
     <t>TEST</t>
   </si>
   <si>
-    <t>Base flow period starts</t>
-  </si>
-  <si>
-    <t>Inundation criteria (partial or complete shoot inundation)</t>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Bed preparation criteria (grading only)</t>
+  </si>
+  <si>
+    <t>Grain size</t>
   </si>
 </sst>
 </file>
@@ -161,7 +170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -276,73 +285,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -356,20 +298,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -384,39 +313,41 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -425,88 +356,103 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,243 +733,281 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="7"/>
-    <col min="3" max="4" width="18.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="3"/>
+    <col min="3" max="3" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="25" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="20"/>
+      <c r="F2" s="38"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="38"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D4" s="29"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="38"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="E5" s="20"/>
+      <c r="F5" s="38"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="15">
+      <c r="B6" s="13"/>
+      <c r="C6" s="31">
         <v>44331</v>
       </c>
-      <c r="D6" s="15">
-        <v>44331</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="D6" s="31"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="38"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="23">
+      <c r="B7" s="13"/>
+      <c r="C7" s="32">
         <v>44378</v>
       </c>
-      <c r="D7" s="23">
-        <v>44378</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+      <c r="D7" s="32"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="38"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="32">
+        <v>44454</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="38"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="33">
+        <v>2</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="38"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="38"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="33">
+        <v>64</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="38"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="38"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="35">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D13" s="35"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="38"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="35">
+        <v>0.03</v>
+      </c>
+      <c r="D14" s="35"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="38"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="35">
+        <v>0</v>
+      </c>
+      <c r="D15" s="35"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="38"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="38"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="36">
+        <v>5</v>
+      </c>
+      <c r="D17" s="36"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="38"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="36">
+        <v>10</v>
+      </c>
+      <c r="D18" s="36"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="38"/>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="23">
-        <v>44454</v>
-      </c>
-      <c r="D8" s="23">
-        <v>44454</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="22">
-        <v>2</v>
-      </c>
-      <c r="D9" s="22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="16">
-        <v>4.7E-2</v>
-      </c>
-      <c r="D11" s="16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="38"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="36">
         <v>14</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="16">
-        <v>0.03</v>
-      </c>
-      <c r="D12" s="16">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="16">
-        <v>0</v>
-      </c>
-      <c r="D13" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="17">
-        <v>5</v>
-      </c>
-      <c r="D15" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="17">
-        <v>10</v>
-      </c>
-      <c r="D16" s="17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="27" t="s">
+      <c r="D20" s="36"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="38"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="17">
-        <v>14</v>
-      </c>
-      <c r="D18" s="17">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="18">
+      <c r="C21" s="37">
         <v>28</v>
       </c>
-      <c r="D19" s="18">
-        <v>28</v>
-      </c>
+      <c r="D21" s="37"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update recruitment template worksheet
</commit_message>
<xml_diff>
--- a/RiparianRecruitment/.templates/recruitment_criteria.xlsx
+++ b/RiparianRecruitment/.templates/recruitment_criteria.xlsx
@@ -754,7 +754,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -966,7 +966,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="36">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="D17" s="36"/>
       <c r="E17" s="25"/>
@@ -980,7 +980,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="36">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D18" s="36"/>
       <c r="E18" s="25"/>
@@ -1041,9 +1041,7 @@
       <c r="B23" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="40">
-        <v>0</v>
-      </c>
+      <c r="C23" s="40"/>
       <c r="D23" s="40"/>
       <c r="E23" s="25"/>
       <c r="F23" s="38"/>
@@ -1055,9 +1053,7 @@
       <c r="B24" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="37">
-        <v>150</v>
-      </c>
+      <c r="C24" s="37"/>
       <c r="D24" s="37"/>
       <c r="E24" s="25"/>
       <c r="F24" s="38"/>

</xml_diff>

<commit_message>
updated worksheet with recruitment band criteria
</commit_message>
<xml_diff>
--- a/RiparianRecruitment/.templates/recruitment_criteria.xlsx
+++ b/RiparianRecruitment/.templates/recruitment_criteria.xlsx
@@ -754,7 +754,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1041,7 +1041,9 @@
       <c r="B23" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="40"/>
+      <c r="C23" s="40">
+        <v>0</v>
+      </c>
       <c r="D23" s="40"/>
       <c r="E23" s="25"/>
       <c r="F23" s="38"/>
@@ -1053,7 +1055,9 @@
       <c r="B24" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="37"/>
+      <c r="C24" s="37">
+        <v>150</v>
+      </c>
       <c r="D24" s="37"/>
       <c r="E24" s="25"/>
       <c r="F24" s="38"/>

</xml_diff>

<commit_message>
update recruitment_criteria.xlsx and corresponding code in criteria class
</commit_message>
<xml_diff>
--- a/RiparianRecruitment/.templates/recruitment_criteria.xlsx
+++ b/RiparianRecruitment/.templates/recruitment_criteria.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Common name</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Lethal inundation</t>
   </si>
   <si>
-    <t>Base flow period starts</t>
-  </si>
-  <si>
     <t>Inundation criteria (partial or complete shoot inundation)</t>
   </si>
   <si>
@@ -111,6 +108,15 @@
     <t>Grain size</t>
   </si>
   <si>
+    <t xml:space="preserve">DO NOT EDIT BELOW </t>
+  </si>
+  <si>
+    <t>BLUE CELLS CAN BE MODIFIED</t>
+  </si>
+  <si>
+    <t>Baseflow period starts</t>
+  </si>
+  <si>
     <t>Recruitment band elevation criteria</t>
   </si>
   <si>
@@ -118,6 +124,9 @@
   </si>
   <si>
     <t xml:space="preserve">cm </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Upper elevation</t>
@@ -185,7 +194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -276,17 +285,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -328,8 +326,10 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -341,6 +341,17 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -348,21 +359,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -371,104 +367,133 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -754,315 +779,319 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="3"/>
-    <col min="3" max="3" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="19" customWidth="1"/>
     <col min="5" max="5" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="38"/>
+      <c r="C1" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="53"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="27" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="38"/>
+      <c r="D2" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="28" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="38"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="30"/>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="29" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="38"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="38"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="30"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="31">
-        <v>44331</v>
-      </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="38"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="24">
+        <v>44683</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="32">
-        <v>44378</v>
-      </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="38"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="25">
+        <v>44746</v>
+      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="30"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="25">
+        <v>44454</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="30"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="26">
+        <v>2</v>
+      </c>
+      <c r="D9" s="26"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="30"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="30"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="26">
+        <v>128</v>
+      </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="30"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="30"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="28">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="30"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="28">
+        <v>0.03</v>
+      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="30"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="28">
+        <v>0</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="30"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="30"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="29">
+        <v>1</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="30"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="29">
+        <v>2.5</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="30"/>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="32">
-        <v>44454</v>
-      </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="38"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="33">
-        <v>2</v>
-      </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="38"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="30"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="29">
+        <v>14</v>
+      </c>
+      <c r="D20" s="33"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="29">
         <v>28</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="38"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="33">
-        <v>128</v>
-      </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="38"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="38"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="35">
-        <v>4.7E-2</v>
-      </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="38"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="35">
-        <v>0.03</v>
-      </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="38"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="35">
-        <v>0</v>
-      </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="38"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="38"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="36">
-        <v>2.5</v>
-      </c>
-      <c r="D17" s="36"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="38"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="36">
-        <v>6</v>
-      </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="38"/>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="38"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="36">
-        <v>14</v>
-      </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="38"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="40">
-        <v>28</v>
-      </c>
-      <c r="D21" s="40"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="38"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="30"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="38"/>
+      <c r="A22" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="40">
-        <v>0</v>
-      </c>
-      <c r="D23" s="40"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="38"/>
+      <c r="A23" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="49"/>
+      <c r="E23"/>
     </row>
     <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="37">
-        <v>150</v>
-      </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="38"/>
+      <c r="A24" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="50"/>
+      <c r="E24"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
revert changes to rec_band handling and update worksheet names
</commit_message>
<xml_diff>
--- a/RiparianRecruitment/.templates/recruitment_criteria.xlsx
+++ b/RiparianRecruitment/.templates/recruitment_criteria.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Common name</t>
   </si>
@@ -30,15 +30,6 @@
     <t>Species</t>
   </si>
   <si>
-    <t>Lifestage</t>
-  </si>
-  <si>
-    <t>Season start</t>
-  </si>
-  <si>
-    <t>Season end</t>
-  </si>
-  <si>
     <t>Fremont Cottonwood</t>
   </si>
   <si>
@@ -48,9 +39,6 @@
     <t>fremontii</t>
   </si>
   <si>
-    <t>Seed Dispersal</t>
-  </si>
-  <si>
     <t>Recession rate criteria</t>
   </si>
   <si>
@@ -126,13 +114,16 @@
     <t xml:space="preserve">cm </t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Upper elevation</t>
   </si>
   <si>
     <t>cm</t>
+  </si>
+  <si>
+    <t>Seed dispersal starts</t>
+  </si>
+  <si>
+    <t>Seed dispersal ends</t>
   </si>
 </sst>
 </file>
@@ -194,7 +185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -326,21 +317,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -367,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -427,9 +403,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -452,13 +425,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -467,7 +434,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -490,10 +456,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -779,7 +751,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,17 +765,17 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="53"/>
+        <v>12</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="51"/>
       <c r="E1" s="14"/>
-      <c r="F1" s="30"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -811,13 +783,13 @@
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="20" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E2" s="14"/>
-      <c r="F2" s="30"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -825,11 +797,11 @@
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="21" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="15"/>
-      <c r="F3" s="30"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
@@ -837,255 +809,241 @@
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="15"/>
-      <c r="F4" s="30"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>9</v>
-      </c>
+      <c r="A5" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="23">
+        <v>44683</v>
+      </c>
+      <c r="D5" s="23"/>
       <c r="E5" s="14"/>
-      <c r="F5" s="30"/>
+      <c r="F5" s="29"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
-        <v>4</v>
+      <c r="A6" s="34" t="s">
+        <v>34</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="24">
-        <v>44683</v>
+        <v>44746</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="16"/>
-      <c r="F6" s="30"/>
+      <c r="F6" s="29"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
-        <v>5</v>
+      <c r="A7" s="35" t="s">
+        <v>27</v>
       </c>
       <c r="B7" s="8"/>
-      <c r="C7" s="25">
-        <v>44746</v>
-      </c>
-      <c r="D7" s="25"/>
+      <c r="C7" s="24">
+        <v>44454</v>
+      </c>
+      <c r="D7" s="24"/>
       <c r="E7" s="16"/>
-      <c r="F7" s="30"/>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="8"/>
+      <c r="A8" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="C8" s="25">
-        <v>44454</v>
+        <v>2</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="16"/>
-      <c r="F8" s="30"/>
+      <c r="F8" s="29"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="26">
-        <v>2</v>
-      </c>
+      <c r="A9" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="26"/>
       <c r="E9" s="17"/>
-      <c r="F9" s="30"/>
+      <c r="F9" s="29"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
+      <c r="A10" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="25">
+        <v>128</v>
+      </c>
+      <c r="D10" s="25"/>
       <c r="E10" s="17"/>
-      <c r="F10" s="30"/>
+      <c r="F10" s="29"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="26">
-        <v>128</v>
-      </c>
+      <c r="A11" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="26"/>
       <c r="E11" s="17"/>
-      <c r="F11" s="30"/>
+      <c r="F11" s="29"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="27"/>
+      <c r="A12" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="27">
+        <v>4.7E-2</v>
+      </c>
       <c r="D12" s="27"/>
       <c r="E12" s="16"/>
-      <c r="F12" s="30"/>
+      <c r="F12" s="29"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="38" t="s">
-        <v>13</v>
+      <c r="A13" s="34" t="s">
+        <v>10</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="28">
-        <v>4.7E-2</v>
-      </c>
-      <c r="D13" s="28"/>
+      <c r="C13" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="D13" s="27"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="30"/>
+      <c r="F13" s="29"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="28">
-        <v>0.03</v>
-      </c>
-      <c r="D14" s="28"/>
+        <v>11</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="27">
+        <v>0</v>
+      </c>
+      <c r="D14" s="27"/>
       <c r="E14" s="18"/>
-      <c r="F14" s="30"/>
+      <c r="F14" s="29"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="28">
-        <v>0</v>
-      </c>
-      <c r="D15" s="28"/>
+      <c r="A15" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="18"/>
-      <c r="F15" s="30"/>
+      <c r="F15" s="29"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="A16" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="28">
+        <v>1</v>
+      </c>
+      <c r="D16" s="28"/>
       <c r="E16" s="19"/>
-      <c r="F16" s="30"/>
+      <c r="F16" s="29"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="29"/>
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="29">
-        <v>1</v>
-      </c>
-      <c r="D17" s="29"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="30"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="29">
-        <v>2.5</v>
-      </c>
-      <c r="D18" s="29"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="19"/>
-      <c r="F18" s="30"/>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="11"/>
+      <c r="F18" s="29"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="28">
+        <v>14</v>
+      </c>
+      <c r="D19" s="31"/>
       <c r="E19" s="19"/>
-      <c r="F19" s="30"/>
+      <c r="F19" s="29"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="29">
-        <v>14</v>
-      </c>
-      <c r="D20" s="33"/>
+      <c r="A20" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="28">
+        <v>28</v>
+      </c>
+      <c r="D20" s="28"/>
       <c r="E20" s="19"/>
-      <c r="F20" s="30"/>
+      <c r="F20" s="29"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="29">
         <v>28</v>
       </c>
-      <c r="D21" s="29"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
       <c r="E21" s="19"/>
-      <c r="F21" s="30"/>
+      <c r="F21" s="29"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="48"/>
+      <c r="D22" s="45"/>
+      <c r="E22"/>
+    </row>
+    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="46"/>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="50"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E24"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update column header from test to template
</commit_message>
<xml_diff>
--- a/RiparianRecruitment/.templates/recruitment_criteria.xlsx
+++ b/RiparianRecruitment/.templates/recruitment_criteria.xlsx
@@ -84,9 +84,6 @@
     <t>Inundation criteria (partial or complete shoot inundation)</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
     <t>mm</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>Seed dispersal ends</t>
+  </si>
+  <si>
+    <t>TEMPLATE</t>
   </si>
 </sst>
 </file>
@@ -751,7 +751,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,13 +765,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="51"/>
       <c r="E1" s="14"/>
@@ -786,7 +786,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="29"/>
@@ -817,7 +817,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="23">
@@ -829,7 +829,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="24">
@@ -841,7 +841,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="24">
@@ -867,7 +867,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="26"/>
@@ -877,10 +877,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="25">
         <v>128</v>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="47"/>
       <c r="C21" s="47"/>
@@ -1023,10 +1023,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="32" t="s">
         <v>29</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>30</v>
       </c>
       <c r="C22" s="48"/>
       <c r="D22" s="45"/>
@@ -1034,10 +1034,10 @@
     </row>
     <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="33" t="s">
         <v>31</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>32</v>
       </c>
       <c r="C23" s="49"/>
       <c r="D23" s="46"/>

</xml_diff>

<commit_message>
update bp raster handling and rr/inund tracking
</commit_message>
<xml_diff>
--- a/RiparianRecruitment/.templates/recruitment_criteria.xlsx
+++ b/RiparianRecruitment/.templates/recruitment_criteria.xlsx
@@ -1,18 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C46BAB9-0FF3-45B1-8D07-C4805808174B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17496" windowHeight="6432"/>
+    <workbookView xWindow="984" yWindow="24" windowWidth="22056" windowHeight="12936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="recruitment" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -129,7 +141,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -343,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -376,22 +388,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -421,36 +430,35 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -747,11 +755,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,291 +767,264 @@
     <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="3"/>
     <col min="3" max="3" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="19" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="3" customWidth="1"/>
     <col min="5" max="5" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="51"/>
+      <c r="D1" s="49"/>
       <c r="E1" s="14"/>
-      <c r="F1" s="29"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="14"/>
-      <c r="F2" s="29"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="21"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="15"/>
-      <c r="F3" s="29"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="21"/>
       <c r="E4" s="15"/>
-      <c r="F4" s="29"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5" s="23">
-        <v>44683</v>
-      </c>
-      <c r="D5" s="23"/>
+      <c r="C5" s="22">
+        <v>45414</v>
+      </c>
+      <c r="D5" s="22"/>
       <c r="E5" s="14"/>
-      <c r="F5" s="29"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="24">
-        <v>44746</v>
-      </c>
-      <c r="D6" s="24"/>
+      <c r="C6" s="23">
+        <v>45463</v>
+      </c>
+      <c r="D6" s="23"/>
       <c r="E6" s="16"/>
-      <c r="F6" s="29"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="35" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="33" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="8"/>
-      <c r="C7" s="24">
-        <v>44454</v>
-      </c>
-      <c r="D7" s="24"/>
+      <c r="C7" s="23">
+        <v>45550</v>
+      </c>
+      <c r="D7" s="23"/>
       <c r="E7" s="16"/>
-      <c r="F7" s="29"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="36" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="34" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="25">
-        <v>2</v>
-      </c>
-      <c r="D8" s="25"/>
+      <c r="C8" s="24">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24"/>
       <c r="E8" s="16"/>
-      <c r="F8" s="29"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="36" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="34" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
       <c r="E9" s="17"/>
-      <c r="F9" s="29"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="35" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="24">
         <v>128</v>
       </c>
-      <c r="D10" s="25"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="17"/>
-      <c r="F10" s="29"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="36" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="34" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="11"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="17"/>
-      <c r="F11" s="29"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="34" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" s="27">
+      <c r="C12" s="26">
         <v>4.7E-2</v>
       </c>
-      <c r="D12" s="27"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="16"/>
-      <c r="F12" s="29"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="34" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="32" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="27">
+      <c r="C13" s="26">
         <v>0.03</v>
       </c>
-      <c r="D13" s="27"/>
+      <c r="D13" s="26"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="29"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="38" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="12"/>
-      <c r="C14" s="27">
+      <c r="C14" s="26">
         <v>0</v>
       </c>
-      <c r="D14" s="27"/>
+      <c r="D14" s="26"/>
       <c r="E14" s="18"/>
-      <c r="F14" s="29"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="39" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="37" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="18"/>
-      <c r="F15" s="29"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="34" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="32" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="28">
-        <v>1</v>
-      </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="29"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="38" t="s">
+      <c r="C16" s="27">
+        <v>3</v>
+      </c>
+      <c r="D16" s="27"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="36" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="28">
-        <v>2.5</v>
-      </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="29"/>
-    </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="40" t="s">
+      <c r="C17" s="27">
+        <v>5</v>
+      </c>
+      <c r="D17" s="27"/>
+    </row>
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="11"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="29"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="41" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="39" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C19" s="27">
         <v>14</v>
       </c>
-      <c r="D19" s="31"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="29"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="38" t="s">
+      <c r="D19" s="29"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="36" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="28">
+      <c r="C20" s="27">
         <v>28</v>
       </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="29"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="42" t="s">
+      <c r="D20" s="27"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="29"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="43" t="s">
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="48"/>
-      <c r="D22" s="45"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="43"/>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="44" t="s">
+    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="46"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="44"/>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E24"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor and final calc updates
</commit_message>
<xml_diff>
--- a/RiparianRecruitment/.templates/recruitment_criteria.xlsx
+++ b/RiparianRecruitment/.templates/recruitment_criteria.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C46BAB9-0FF3-45B1-8D07-C4805808174B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74DB126-1298-428B-8DAC-B666B0B65B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="984" yWindow="24" windowWidth="22056" windowHeight="12936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1308" yWindow="384" windowWidth="21732" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="recruitment" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Common name</t>
   </si>
@@ -60,15 +60,6 @@
     <t>Bed shear stress criteria</t>
   </si>
   <si>
-    <t>Prepared</t>
-  </si>
-  <si>
-    <t>Partially prepared</t>
-  </si>
-  <si>
-    <t>Unprepared</t>
-  </si>
-  <si>
     <t>UNITS</t>
   </si>
   <si>
@@ -136,6 +127,12 @@
   </si>
   <si>
     <t>TEMPLATE</t>
+  </si>
+  <si>
+    <t>Fully mobilized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partially mobilized </t>
   </si>
 </sst>
 </file>
@@ -759,7 +756,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -773,13 +770,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D1" s="49"/>
       <c r="E1" s="14"/>
@@ -793,7 +790,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E2" s="14"/>
     </row>
@@ -821,7 +818,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="22">
@@ -832,7 +829,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="23">
@@ -843,21 +840,21 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="23">
-        <v>45550</v>
+        <v>45474</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="16"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8" s="24">
         <v>1</v>
@@ -867,7 +864,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="25"/>
@@ -876,10 +873,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="24">
         <v>128</v>
@@ -898,7 +895,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="26">
@@ -908,8 +905,8 @@
       <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="32" t="s">
-        <v>10</v>
+      <c r="A13" s="36" t="s">
+        <v>33</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="26">
@@ -919,109 +916,101 @@
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="26">
-        <v>0</v>
-      </c>
-      <c r="D14" s="26"/>
+      <c r="A14" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
+      <c r="A15" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="27">
+        <v>2.5</v>
+      </c>
+      <c r="D15" s="27"/>
       <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="27">
+        <v>5</v>
+      </c>
+      <c r="D16" s="27"/>
+    </row>
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="27">
+        <v>14</v>
+      </c>
+      <c r="D18" s="29"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="27">
-        <v>3</v>
-      </c>
-      <c r="D16" s="27"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="27">
-        <v>5</v>
-      </c>
-      <c r="D17" s="27"/>
-    </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>13</v>
+      <c r="B19" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="C19" s="27">
-        <v>14</v>
-      </c>
-      <c r="D19" s="29"/>
+        <v>28</v>
+      </c>
+      <c r="D19" s="27"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="27">
+      <c r="A20" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="46"/>
+      <c r="D21" s="43"/>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="27"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="46"/>
-      <c r="D22" s="43"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="44"/>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="44"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E23"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>